<commit_message>
qto-200902212159 add an hierarchy table reloading shell action
</commit_message>
<xml_diff>
--- a/dat/xls/styler.xlsx
+++ b/dat/xls/styler.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ysg/opt/qto/qto.0.8.5.dev.ysg@host-name/dat/xls/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ysg/opt/qto/qto.0.8.6.dev.ysg@host-name/dat/mix/2020/2020-08/2020-08-24/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CD54E2-5E14-8542-9A31-60A7A5C80783}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5636CC-C014-C14C-9555-4B03A5166D52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="table_name" sheetId="3" r:id="rId1"/>
-    <sheet name="table_name_02" sheetId="6" r:id="rId2"/>
+    <sheet name="test_hierarchy_doc" sheetId="7" r:id="rId1"/>
+    <sheet name="styler" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
   <si>
     <t>level</t>
   </si>
@@ -72,21 +72,6 @@
     <t>07-qas</t>
   </si>
   <si>
-    <t>issue-tracker-design</t>
-  </si>
-  <si>
-    <t>03-act</t>
-  </si>
-  <si>
-    <t>2017-12-31</t>
-  </si>
-  <si>
-    <t>2017-03-01</t>
-  </si>
-  <si>
-    <t>achieve simplistic design and ease to use</t>
-  </si>
-  <si>
     <t>seq</t>
   </si>
   <si>
@@ -162,25 +147,93 @@
     <t>2017-08-20 11:00</t>
   </si>
   <si>
-    <t>goal</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>formats</t>
+  </si>
+  <si>
+    <t>src</t>
+  </si>
+  <si>
+    <t>rgt</t>
+  </si>
+  <si>
+    <t>lft</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>guid</t>
+  </si>
+  <si>
+    <t>e58baecb-4530-4e2a-b948-2072fff0bbcc</t>
+  </si>
+  <si>
+    <t>f3bad87a-8e7f-4842-9458-7b4aad29b4e0</t>
+  </si>
+  <si>
+    <t>0d42a4d9-81de-4e47-a540-46928e2ee042</t>
+  </si>
+  <si>
+    <t>0a48d2f0-3baa-473e-bf04-955228e78b3f</t>
+  </si>
+  <si>
+    <t>787b280a-0c2b-4cc8-a189-3ae5748ddf53</t>
+  </si>
+  <si>
+    <t>f2292d70-a0cf-44be-9159-f84447f61a6f</t>
+  </si>
+  <si>
+    <t>79d93e14-c3f3-4e81-956d-5ac8596aeffa</t>
+  </si>
+  <si>
+    <t>2,2 title</t>
+  </si>
+  <si>
+    <t>2.1. title</t>
+  </si>
+  <si>
+    <t>1,2 title</t>
+  </si>
+  <si>
+    <t>0 - THE ROOT</t>
+  </si>
+  <si>
+    <t>1.1. title</t>
+  </si>
+  <si>
+    <t>21bb170a-03ac-4358-832f-fd3d0f3ff176</t>
+  </si>
+  <si>
+    <t>1.1.2 title</t>
+  </si>
+  <si>
+    <t>2f94ce92-8c52-432d-98ad-949467f01841</t>
+  </si>
+  <si>
+    <t>1.1.1 title</t>
+  </si>
+  <si>
+    <t>2.0 TITLE</t>
+  </si>
+  <si>
+    <t>1.0 TITLE</t>
+  </si>
+  <si>
+    <t>8ba2f97e-24d3-434a-b8c8-d745aafcc1a2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -193,13 +246,6 @@
       <color rgb="FF3D3D3D"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -217,14 +263,9 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -308,79 +349,71 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="22" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="22" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" applyProtection="0">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="0">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="4">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="3">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="5" applyFill="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="4" applyFill="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="5">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="4">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="6">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="5">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="6" applyFill="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="5" applyFill="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="6">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="3" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="5" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="7">
     <cellStyle name="Accent1" xfId="1" builtinId="29" customBuiltin="1"/>
     <cellStyle name="DateStyle" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="decimal" xfId="8" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="HeadersStyle" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="HeadingStyle" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="decimal" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="HeadingStyle" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Normal 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 3" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="TextStyle" xfId="5" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="WholeNumberStyle" xfId="6" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="TextStyle" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="WholeNumberStyle" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -415,24 +448,6 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="actual_hours" dataCellStyle="decimal"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="owner" dataCellStyle="TextStyle"/>
     <tableColumn id="10" xr3:uid="{F283BC6C-4938-4069-8058-8BFB26B9748F}" name="type" dataCellStyle="TextStyle"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table136" displayName="Table136" ref="A1:J2" totalsRowShown="0" headerRowCellStyle="HeadingStyle" dataCellStyle="TextStyle">
-  <tableColumns count="10">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="level" dataCellStyle="WholeNumberStyle"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="prio" dataCellStyle="WholeNumberStyle"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="status" dataCellStyle="TextStyle"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="category" dataCellStyle="TextStyle"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="name" dataCellStyle="TextStyle"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="description" dataCellStyle="TextStyle"/>
-    <tableColumn id="13" xr3:uid="{000FD16E-28D2-41E0-9692-5F700D6679FF}" name="type" dataCellStyle="TextStyle"/>
-    <tableColumn id="10" xr3:uid="{236EE40F-F6E1-4482-A766-6CB0C0BC7B4C}" name="owner" dataCellStyle="TextStyle"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="start_time" dataCellStyle="TextStyle"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="stop_time" dataCellStyle="TextStyle"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -758,14 +773,333 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D0073C-B782-1845-B845-60DC55E1C76B}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="38" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="32.1640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="19.5" style="6" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="22.5" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="4">
+        <v>200726094848</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4">
+        <v>200726101948</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="4">
+        <v>200824052219</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4">
+        <v>5</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="4">
+        <v>200824052531</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4">
+        <v>6</v>
+      </c>
+      <c r="F6" s="4">
+        <v>7</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="4">
+        <v>200824052420</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4">
+        <v>8</v>
+      </c>
+      <c r="F7" s="4">
+        <v>9</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="4">
+        <v>200726102001</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>7</v>
+      </c>
+      <c r="E8" s="4">
+        <v>11</v>
+      </c>
+      <c r="F8" s="4">
+        <v>12</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="4">
+        <v>200824045752</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4">
+        <v>14</v>
+      </c>
+      <c r="F9" s="4">
+        <v>19</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="4">
+        <v>200824051810</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4">
+        <v>15</v>
+      </c>
+      <c r="F10" s="4">
+        <v>16</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="4">
+        <v>200824051818</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>10</v>
+      </c>
+      <c r="E11" s="4">
+        <v>17</v>
+      </c>
+      <c r="F11" s="4">
+        <v>18</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J11">
+    <sortCondition ref="D6"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="3" width="5.6640625" style="6" customWidth="1"/>
     <col min="4" max="6" width="12.6640625" style="6" customWidth="1"/>
@@ -776,12 +1110,12 @@
     <col min="12" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -790,7 +1124,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -808,19 +1142,19 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -831,25 +1165,25 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K2" s="7">
         <v>4</v>
@@ -861,10 +1195,10 @@
         <v>9</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -875,19 +1209,19 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -901,10 +1235,10 @@
         <v>9</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -915,25 +1249,25 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="K4" s="7">
         <f>80/60</f>
@@ -946,10 +1280,10 @@
         <v>9</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -963,22 +1297,22 @@
         <v>11</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="K5" s="14">
         <v>1.33</v>
@@ -990,10 +1324,10 @@
         <v>9</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="11">
         <v>1</v>
       </c>
@@ -1007,22 +1341,22 @@
         <v>12</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="K6" s="15">
         <v>1.33</v>
@@ -1034,99 +1368,7 @@
         <v>9</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="2" width="5.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" customWidth="1"/>
-    <col min="6" max="6" width="36.6640625" customWidth="1"/>
-    <col min="7" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="10" width="12.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="4">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>